<commit_message>
added chart for recursively collecting match data on civs
</commit_message>
<xml_diff>
--- a/AoE2_tabular.xlsx
+++ b/AoE2_tabular.xlsx
@@ -94,12 +94,12 @@
     <t>76561198400058723</t>
   </si>
   <si>
+    <t>76561198135964589</t>
+  </si>
+  <si>
     <t>76561199014239939</t>
   </si>
   <si>
-    <t>76561198135964589</t>
-  </si>
-  <si>
     <t>76561198044559189</t>
   </si>
   <si>
@@ -394,10 +394,10 @@
     <t>GL.JorDan_AoE</t>
   </si>
   <si>
+    <t>GL.slam</t>
+  </si>
+  <si>
     <t>CELTS</t>
-  </si>
-  <si>
-    <t>GL.slam</t>
   </si>
   <si>
     <t>GL.DauT</t>
@@ -4006,7 +4006,7 @@
     </row>
     <row r="29" spans="2:8">
       <c r="B29">
-        <v>2400</v>
+        <v>2405</v>
       </c>
       <c r="C29" t="s">
         <v>25</v>
@@ -4015,21 +4015,21 @@
         <v>125</v>
       </c>
       <c r="E29" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="F29">
-        <v>3922</v>
+        <v>3275</v>
       </c>
       <c r="G29">
-        <v>2232</v>
+        <v>1964</v>
       </c>
       <c r="H29">
-        <v>1690</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="30" spans="2:8">
       <c r="B30">
-        <v>2398</v>
+        <v>2400</v>
       </c>
       <c r="C30" t="s">
         <v>26</v>
@@ -4038,16 +4038,16 @@
         <v>126</v>
       </c>
       <c r="E30" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="F30">
-        <v>3274</v>
+        <v>3922</v>
       </c>
       <c r="G30">
-        <v>1963</v>
+        <v>2232</v>
       </c>
       <c r="H30">
-        <v>1311</v>
+        <v>1690</v>
       </c>
     </row>
     <row r="31" spans="2:8">
@@ -4995,7 +4995,7 @@
     </row>
     <row r="72" spans="2:8">
       <c r="B72">
-        <v>2264</v>
+        <v>2257</v>
       </c>
       <c r="C72" t="s">
         <v>68</v>
@@ -5007,13 +5007,13 @@
         <v>226</v>
       </c>
       <c r="F72">
-        <v>2471</v>
+        <v>2472</v>
       </c>
       <c r="G72">
         <v>1340</v>
       </c>
       <c r="H72">
-        <v>1131</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="73" spans="2:8">

</xml_diff>